<commit_message>
Saved transition-level IA xlsx file for mangroves
</commit_message>
<xml_diff>
--- a/3 mmr land cover transitions/mangroves/intensity analysis/macros/Transition_Level_Intensity_Analysis.xlsx
+++ b/3 mmr land cover transitions/mangroves/intensity analysis/macros/Transition_Level_Intensity_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dondealban/Dropbox/Research/myanmar/3 mmr land cover transitions/mangroves/intensity analysis/macros/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3971AC37-10BE-264B-BE12-1FCDBB257DB5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA76E32-CC16-AF4E-9B2C-EE9E2F38B9D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{026BCF9A-6539-7B40-A798-30841E138290}"/>
   </bookViews>
@@ -653,7 +653,7 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -688,7 +688,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -723,7 +723,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -758,7 +758,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -793,7 +793,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -828,7 +828,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -863,7 +863,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -898,7 +898,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -933,7 +933,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>0.18025653064250946</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>19</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -1948,7 +1948,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>19</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>19</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>19</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>19</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>26</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
         <v>26</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
         <v>26</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
         <v>26</v>
       </c>
@@ -2508,7 +2508,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
         <v>26</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
         <v>26</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
         <v>26</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
         <v>26</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
         <v>26</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>0.20010806620121002</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
         <v>26</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>0.20010802149772644</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
         <v>26</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>0.20010806620121002</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="18" t="s">
         <v>26</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>0.20010802149772644</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="18" t="s">
         <v>26</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>0.20010802149772644</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="18" t="s">
         <v>26</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>0.20010806620121002</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="18" t="s">
         <v>26</v>
       </c>
@@ -2893,7 +2893,7 @@
         <v>0.20010806620121002</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="18" t="s">
         <v>26</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>0.20010802149772644</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="18" t="s">
         <v>26</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="18" t="s">
         <v>26</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="18" t="s">
         <v>26</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="18" t="s">
         <v>26</v>
       </c>
@@ -3068,7 +3068,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="18" t="s">
         <v>26</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="18" t="s">
         <v>26</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="18" t="s">
         <v>26</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="18" t="s">
         <v>26</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="18" t="s">
         <v>26</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="18" t="s">
         <v>26</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="18" t="s">
         <v>26</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="18" t="s">
         <v>26</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="18" t="s">
         <v>26</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="18" t="s">
         <v>26</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="18" t="s">
         <v>26</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="18" t="s">
         <v>26</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="18" t="s">
         <v>26</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="18" t="s">
         <v>26</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="18" t="s">
         <v>26</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="18" t="s">
         <v>26</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="86" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="18" t="s">
         <v>26</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="87" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="18" t="s">
         <v>26</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="88" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="18" t="s">
         <v>26</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="89" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="18" t="s">
         <v>26</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="18" t="s">
         <v>26</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="91" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
         <v>26</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="18" t="s">
         <v>26</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="18" t="s">
         <v>26</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="94" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="18" t="s">
         <v>26</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="18" t="s">
         <v>26</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="18" t="s">
         <v>26</v>
       </c>
@@ -4013,7 +4013,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="18" t="s">
         <v>26</v>
       </c>
@@ -4076,7 +4076,7 @@
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>0.28898504376411438</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>19</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>19</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>19</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>19</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>19</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>26</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
         <v>26</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
         <v>26</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
         <v>26</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
         <v>26</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
         <v>26</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="18" t="s">
         <v>26</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
         <v>26</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
         <v>26</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
         <v>26</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="18" t="s">
         <v>26</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="18" t="s">
         <v>26</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="18" t="s">
         <v>26</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="18" t="s">
         <v>26</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="18" t="s">
         <v>26</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="18" t="s">
         <v>26</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="18" t="s">
         <v>26</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>0.1431262344121933</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="18" t="s">
         <v>26</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>0.1431262344121933</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="18" t="s">
         <v>26</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>0.1431262344121933</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="18" t="s">
         <v>26</v>
       </c>
@@ -6491,7 +6491,7 @@
         <v>0.1431262344121933</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="18" t="s">
         <v>26</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>0.1431262344121933</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="18" t="s">
         <v>26</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>0.1431262344121933</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="18" t="s">
         <v>26</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>0.1431262344121933</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="18" t="s">
         <v>26</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>0.1431262344121933</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="18" t="s">
         <v>26</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="18" t="s">
         <v>26</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="18" t="s">
         <v>26</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="18" t="s">
         <v>26</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="18" t="s">
         <v>26</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="18" t="s">
         <v>26</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="18" t="s">
         <v>26</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="18" t="s">
         <v>26</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="82" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="18" t="s">
         <v>26</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="83" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="18" t="s">
         <v>26</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="18" t="s">
         <v>26</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="85" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="18" t="s">
         <v>26</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="86" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="18" t="s">
         <v>26</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="87" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="18" t="s">
         <v>26</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="88" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="18" t="s">
         <v>26</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="89" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="18" t="s">
         <v>26</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="90" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="18" t="s">
         <v>26</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="91" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
         <v>26</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="92" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="18" t="s">
         <v>26</v>
       </c>
@@ -7296,7 +7296,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="18" t="s">
         <v>26</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="94" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="18" t="s">
         <v>26</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="95" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="18" t="s">
         <v>26</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="96" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="18" t="s">
         <v>26</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="97" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="18" t="s">
         <v>26</v>
       </c>

</xml_diff>